<commit_message>
feat: Mejorar la vista de empresa con información detallada y botones de administración
</commit_message>
<xml_diff>
--- a/resources/utils/TABLA DE PERMISOS.xlsx
+++ b/resources/utils/TABLA DE PERMISOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CURSOS DEV\PROJECTS\DinamyLAB\resources\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514146AD-13EB-40D7-9CDB-5AA281554AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC53A084-0A2B-426D-ADD1-E08980A6B495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F46AA0C-A919-44D0-B019-12E003187D24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F46AA0C-A919-44D0-B019-12E003187D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>ADMINISTRADOR</t>
   </si>
@@ -85,13 +85,37 @@
   </si>
   <si>
     <t>*que es ver resultado</t>
+  </si>
+  <si>
+    <t>CONFIGURACIÓN</t>
+  </si>
+  <si>
+    <t>EMPRESA</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>SEDES</t>
+  </si>
+  <si>
+    <t>EMPLEADOS</t>
+  </si>
+  <si>
+    <t>CONVENIOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,8 +123,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +178,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -155,11 +213,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -174,8 +399,66 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,10 +474,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +532,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -338,7 +638,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,7 +780,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2303AF-7A9A-4574-B83C-41CBDC438E8A}">
-  <dimension ref="B2:J16"/>
+  <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,9 +962,228 @@
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
     </row>
+    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>